<commit_message>
add result.xlsx and robert lstm result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747C164-FBCB-4046-9AB8-0A6A65F9550C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25136D-B7BD-478B-8ABF-B5AE1AED332A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="184" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -127,7 +127,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -410,19 +410,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -477,7 +478,7 @@
         <v>0.55370066760532299</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -506,7 +507,7 @@
         <v>0.54521530433132903</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -535,7 +536,7 @@
         <v>0.50335322298542595</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -575,20 +576,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03916FF-E967-4F88-8D67-A577C87F376D}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -643,7 +644,7 @@
         <v>0.55261347947983797</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -672,7 +673,7 @@
         <v>0.53205009429244798</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -701,7 +702,7 @@
         <v>0.45742061963469099</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
udpate roberta lstm baseline result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25136D-B7BD-478B-8ABF-B5AE1AED332A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DC6F78-6C87-4D4B-B7A4-D6D1ABDF975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,10 @@
   </si>
   <si>
     <t>bert + lstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roberta + lstm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,15 +578,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03916FF-E967-4F88-8D67-A577C87F376D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
@@ -731,6 +735,35 @@
         <v>0.54720000000000002</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.4501999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.30430000000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.31640000000000001</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.54590000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update roberta + cnn and bert + bilstm result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DC6F78-6C87-4D4B-B7A4-D6D1ABDF975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52B8EA5-6E86-4757-8DC3-98DB07A1A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,22 @@
   </si>
   <si>
     <t>roberta + lstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deberta + lstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bert + cnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>robert + cnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bert + bilstm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,161 +428,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>1.4800509423058501</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0.66685660970327298</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0.64409568637525105</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.66685660970327298</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.63908635347585596</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>0.32164394597309198</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>0.32397533647661603</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0.55370066760532299</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>1.44975102880273</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.66058332477787796</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.63558093552992301</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.66058332477787796</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.63045577316712098</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0.30715774214506403</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>0.313187131023001</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.54521530433132903</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>1.58270289828581</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.64255996652048497</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.59080816764147304</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.64255996652048497</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.59583838432570702</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>0.27586856566350298</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>0.27781512936733999</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.50335322298542595</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1.4539</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>0.66390000000000005</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>0.63580000000000003</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.66390000000000005</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.63270000000000004</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.31879999999999997</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>0.32179999999999997</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>0.54830000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.4501999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.30430000000000001</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.31640000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.54590000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.4902000000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.46920000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.46920000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.30409999999999998</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.52E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.18E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.5245</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.68240000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.67849999999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.41959999999999997</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.42309999999999998</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.4946999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.68710000000000004</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.40720000000000001</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.40849999999999997</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.58109999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.5226</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.68220000000000003</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.6845</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.68220000000000003</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.40410000000000001</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.58230000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -578,22 +782,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03916FF-E967-4F88-8D67-A577C87F376D}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -648,7 +852,7 @@
         <v>0.55261347947983797</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -677,7 +881,7 @@
         <v>0.53205009429244798</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -706,7 +910,7 @@
         <v>0.45742061963469099</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -733,39 +937,11 @@
       </c>
       <c r="I5" s="2">
         <v>0.54720000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.4501999999999999</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.65380000000000005</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.64070000000000005</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.65380000000000005</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.63419999999999999</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.30430000000000001</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.31640000000000001</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.54590000000000005</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update deberta + cnn
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52B8EA5-6E86-4757-8DC3-98DB07A1A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B2C7D6-714A-4A82-BC81-8518F7E26BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,10 @@
   </si>
   <si>
     <t>bert + bilstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deberta + cnn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -431,7 +435,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -729,6 +733,33 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.7863</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.58660000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.58989999999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.31240000000000001</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.47110000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update roberta + bilstm result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B2C7D6-714A-4A82-BC81-8518F7E26BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DDC3BA-FD4A-4DAE-A16E-46BEBDE80247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +96,10 @@
   </si>
   <si>
     <t>deberta + cnn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roberta + bilstm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,13 +439,13 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -797,6 +801,33 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.5179</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.66920000000000002</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.66920000000000002</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.65590000000000004</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.37390000000000001</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.37919999999999998</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.56730000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
udpate bert + lstm
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DDC3BA-FD4A-4DAE-A16E-46BEBDE80247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1CE7F5-304D-4FE2-BE79-7CE87B07EA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>roberta + bilstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deberta + bilstm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 hrs 44 mins 30 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -450,9 +462,10 @@
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +490,11 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -510,7 +526,7 @@
         <v>0.55370066760532299</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -542,7 +558,7 @@
         <v>0.54521530433132903</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -574,7 +590,7 @@
         <v>0.50335322298542595</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -582,31 +598,34 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1.4539</v>
+        <v>1.4444999999999999</v>
       </c>
       <c r="D5" s="2">
-        <v>0.66390000000000005</v>
+        <v>0.67720000000000002</v>
       </c>
       <c r="E5" s="2">
-        <v>0.63580000000000003</v>
+        <v>0.67520000000000002</v>
       </c>
       <c r="F5" s="2">
-        <v>0.66390000000000005</v>
+        <v>0.67720000000000002</v>
       </c>
       <c r="G5" s="2">
-        <v>0.63270000000000004</v>
+        <v>0.66369999999999996</v>
       </c>
       <c r="H5" s="2">
-        <v>0.31879999999999997</v>
+        <v>0.374</v>
       </c>
       <c r="I5" s="2">
-        <v>0.32179999999999997</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="J5" s="2">
-        <v>0.54830000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.57569999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -638,7 +657,7 @@
         <v>0.54590000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -670,7 +689,7 @@
         <v>2.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -702,7 +721,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -734,7 +753,7 @@
         <v>0.58109999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -766,7 +785,7 @@
         <v>0.47110000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -798,7 +817,7 @@
         <v>0.58230000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -830,9 +849,36 @@
         <v>0.56730000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.2258</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.30330000000000001</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.2700000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update roberta/deberta + lstim/bilstm result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1CE7F5-304D-4FE2-BE79-7CE87B07EA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7077C92C-3AF1-413E-832B-577940923EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,42 @@
   </si>
   <si>
     <t>total time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 hrs 41 mins 41 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 hrs 40 mins 59 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 hrs 8 mins 46 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 hrs 41 mins 55 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 hrs 29 mins 3 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 hrs 46 mins 19 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 hrs 5 mins 20 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13 hrs 8 mins 24 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 hrs 59 mins 34 secs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -172,7 +208,64 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -451,7 +544,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -502,28 +595,31 @@
         <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>1.4800509423058501</v>
+        <v>1.5407</v>
       </c>
       <c r="D2" s="2">
-        <v>0.66685660970327298</v>
+        <v>0.68120000000000003</v>
       </c>
       <c r="E2" s="2">
-        <v>0.64409568637525105</v>
+        <v>0.68869999999999998</v>
       </c>
       <c r="F2" s="2">
-        <v>0.66685660970327298</v>
+        <v>0.68120000000000003</v>
       </c>
       <c r="G2" s="2">
-        <v>0.63908635347585596</v>
+        <v>0.67110000000000003</v>
       </c>
       <c r="H2" s="2">
-        <v>0.32164394597309198</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="I2" s="2">
-        <v>0.32397533647661603</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="J2" s="2">
-        <v>0.55370066760532299</v>
+        <v>0.58140000000000003</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -656,6 +752,9 @@
       <c r="J6" s="2">
         <v>0.54590000000000005</v>
       </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -688,6 +787,9 @@
       <c r="J7" s="2">
         <v>2.8400000000000002E-2</v>
       </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -720,6 +822,9 @@
       <c r="J8" s="2">
         <v>0.57599999999999996</v>
       </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -752,6 +857,9 @@
       <c r="J9" s="2">
         <v>0.58109999999999995</v>
       </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -784,6 +892,9 @@
       <c r="J10" s="2">
         <v>0.47110000000000002</v>
       </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -816,6 +927,9 @@
       <c r="J11" s="2">
         <v>0.58230000000000004</v>
       </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -848,6 +962,9 @@
       <c r="J12" s="2">
         <v>0.56730000000000003</v>
       </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -880,9 +997,36 @@
       <c r="J13" s="2">
         <v>2.2700000000000001E-2</v>
       </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C2:C13">
+    <cfRule type="top10" dxfId="7" priority="8" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
+    <cfRule type="top10" dxfId="6" priority="7" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="top10" dxfId="5" priority="6" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F13">
+    <cfRule type="top10" dxfId="4" priority="5" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="top10" dxfId="3" priority="4" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
+    <cfRule type="top10" dxfId="2" priority="3" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I13">
+    <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J13">
+    <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update ros 01~05 result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7077C92C-3AF1-413E-832B-577940923EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3822F27C-0FED-47B8-BFFB-09544F25A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-60" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update ros deberta + lstm result and use 5 fold
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3822F27C-0FED-47B8-BFFB-09544F25A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C567E8-EA2A-4888-A7B0-0DA88D7FE025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,6 +148,38 @@
   </si>
   <si>
     <t>3 hrs 59 mins 34 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 hrs 54 mins 34 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 hrs 22 mins 39 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11 hrs 38 mins 41 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 hrs 40 mins 24 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 hrs 12 mins 1 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 hrs 31 mins 35 secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>世哲電腦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 hrs 30 mins 41 secs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1034,161 +1066,337 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03916FF-E967-4F88-8D67-A577C87F376D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.4694101314607799</v>
-      </c>
       <c r="C2" s="2">
-        <v>0.66471954890899199</v>
+        <v>1.4964</v>
       </c>
       <c r="D2" s="2">
-        <v>0.66299791445706502</v>
+        <v>0.66259999999999997</v>
       </c>
       <c r="E2" s="2">
-        <v>0.66471954890899199</v>
+        <v>0.68520000000000003</v>
       </c>
       <c r="F2" s="2">
-        <v>0.64502046722677098</v>
+        <v>0.66259999999999997</v>
       </c>
       <c r="G2" s="2">
-        <v>0.38213813781948403</v>
+        <v>0.65949999999999998</v>
       </c>
       <c r="H2" s="2">
-        <v>0.39326876343502098</v>
+        <v>0.43130000000000002</v>
       </c>
       <c r="I2" s="2">
-        <v>0.55261347947983797</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>0.45019999999999999</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.56540000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.44505114076713</v>
-      </c>
       <c r="C3" s="2">
-        <v>0.64805017169032597</v>
+        <v>1.5556000000000001</v>
       </c>
       <c r="D3" s="2">
-        <v>0.64990819754797102</v>
+        <v>0.65239999999999998</v>
       </c>
       <c r="E3" s="2">
-        <v>0.64805017169032597</v>
+        <v>0.68389999999999995</v>
       </c>
       <c r="F3" s="2">
-        <v>0.62831015417420999</v>
+        <v>0.65239999999999998</v>
       </c>
       <c r="G3" s="2">
-        <v>0.36539890077612203</v>
+        <v>0.6542</v>
       </c>
       <c r="H3" s="2">
-        <v>0.39019583807958502</v>
+        <v>0.41489999999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.53205009429244798</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.55410000000000004</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
-        <v>1.6792079284841499</v>
-      </c>
       <c r="C4" s="2">
-        <v>0.62481283255751296</v>
+        <v>2.0638000000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>0.58890893891412599</v>
+        <v>0.58709999999999996</v>
       </c>
       <c r="E4" s="2">
-        <v>0.62481283255751296</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="F4" s="2">
-        <v>0.58428923251136</v>
+        <v>0.58709999999999996</v>
       </c>
       <c r="G4" s="2">
-        <v>0.30716468986260598</v>
+        <v>0.54279999999999995</v>
       </c>
       <c r="H4" s="2">
-        <v>0.32445532069253202</v>
+        <v>0.2777</v>
       </c>
       <c r="I4" s="2">
-        <v>0.45742061963469099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>0.2974</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.38779999999999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>1.4300999999999999</v>
-      </c>
       <c r="C5" s="2">
-        <v>0.66249999999999998</v>
+        <v>1.45</v>
       </c>
       <c r="D5" s="2">
-        <v>0.65429999999999999</v>
+        <v>0.65739999999999998</v>
       </c>
       <c r="E5" s="2">
-        <v>0.66249999999999998</v>
+        <v>0.67730000000000001</v>
       </c>
       <c r="F5" s="2">
-        <v>0.6391</v>
+        <v>0.65739999999999998</v>
       </c>
       <c r="G5" s="2">
-        <v>0.37659999999999999</v>
+        <v>0.6522</v>
       </c>
       <c r="H5" s="2">
-        <v>0.38700000000000001</v>
+        <v>0.41489999999999999</v>
       </c>
       <c r="I5" s="2">
-        <v>0.54720000000000002</v>
+        <v>0.43990000000000001</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.55549999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.4863999999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.626</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.626</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.62439999999999996</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.38669999999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.52080000000000004</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.9390999999999998</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.46710000000000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.22439999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.46710000000000002</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.30270000000000002</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.5187999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.66149999999999998</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.42630000000000001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.44290000000000002</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.56720000000000004</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add word2vec + eda
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5784CBA-1DEA-41FD-9E4B-2BBD52C87340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343CB33C-029B-45E5-8508-79AA51BC99AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="resampling" sheetId="2" r:id="rId4"/>
     <sheet name="48label_baseline" sheetId="5" r:id="rId5"/>
     <sheet name="48label_ros" sheetId="6" r:id="rId6"/>
+    <sheet name="48label_word2vec" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -579,6 +580,42 @@
   </si>
   <si>
     <t>1 hrs 19 mins 13 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 46 mins 16 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 45 mins 8 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 3 mins 3 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 48 mins 14 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 5 mins 50 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 5 mins 47 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 13 mins 14 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 32 mins 41 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 52 mins 47 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 5 mins 15 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 53 mins 35 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 16 mins 4 secs</t>
   </si>
 </sst>
 </file>
@@ -662,7 +699,14 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1760,34 +1804,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="34" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="35" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="33" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="34" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="32" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="33" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="31" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="32" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="30" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="31" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="29" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="30" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="28" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="29" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="27" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="28" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="26" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="27" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="25" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="26" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1798,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098E111A-5A85-461C-839C-9C5105448BDD}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2314,16 +2358,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B25">
-    <cfRule type="top10" dxfId="24" priority="4" rank="5"/>
+    <cfRule type="top10" dxfId="25" priority="4" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="top10" dxfId="23" priority="3" rank="5"/>
+    <cfRule type="top10" dxfId="24" priority="3" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F25">
-    <cfRule type="top10" dxfId="22" priority="2" rank="5"/>
+    <cfRule type="top10" dxfId="23" priority="2" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G25">
-    <cfRule type="top10" dxfId="21" priority="1" rank="5"/>
+    <cfRule type="top10" dxfId="22" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2774,10 +2818,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="20" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="21" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="19" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="20" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3359,34 +3403,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="18" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="19" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="17" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="18" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="16" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="17" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="15" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="16" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="14" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="15" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="13" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="14" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="12" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="13" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="11" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="12" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="10" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="11" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="9" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3910,25 +3954,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="8" priority="7" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="9" priority="7" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="7" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="8" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="6" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="7" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="5" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="6" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="4" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="5" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="3" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="4" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="2" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="3" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3940,7 +3984,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4417,8 +4461,499 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="2" rank="3"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E03F8-CCBA-4CA7-B914-11C40186E5A7}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1.8025</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.63619999999999999</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.64449999999999996</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.63619999999999999</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.62970000000000004</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.4234</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.42030000000000001</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.52249999999999996</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.25929999999999997</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.7537</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.65069999999999995</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.6462</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.65069999999999995</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.63790000000000002</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.43090000000000001</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.42770000000000002</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.53449999999999998</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.6760999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.64490000000000003</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.63929999999999998</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.64490000000000003</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.63129999999999997</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.41770000000000002</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.52380000000000004</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.27260000000000001</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.5810999999999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.65480000000000005</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.64590000000000003</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.65480000000000005</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.63829999999999998</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.41539999999999999</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.40379999999999999</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.37169999999999997</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1.9300999999999999</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.6411</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.6421</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.6411</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.63260000000000005</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.41820000000000002</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.42049999999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.52569999999999995</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.1636</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.8488</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.64049999999999996</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.64449999999999996</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.64049999999999996</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.63249999999999995</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.41460000000000002</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.52549999999999997</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.17119999999999999</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.60909999999999997</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.61570000000000003</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.60909999999999997</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.59260000000000002</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.3735</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.3952</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.4748</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.7036</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.8138000000000001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.59460000000000002</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.61850000000000005</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.59460000000000002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.59079999999999999</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.38159999999999999</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.39510000000000001</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.4708</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.44080000000000003</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2.0933999999999999</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.58509999999999995</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.55069999999999997</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.58509999999999995</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.33289999999999997</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.40150000000000002</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.97460000000000002</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.214</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.6008</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.55269999999999997</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.6008</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.56059999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.32879999999999998</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.32550000000000001</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.41310000000000002</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.8306</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2.4234</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.46829999999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.3589</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.46829999999999999</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="G12" s="4">
+        <v>6.59E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>9.69E-2</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.221</v>
+      </c>
+      <c r="J12" s="5">
+        <v>2.8668999999999998</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2.3544999999999998</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.4965</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.41360000000000002</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.4965</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.43380000000000002</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.12989999999999999</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.27560000000000001</v>
+      </c>
+      <c r="J13" s="5">
+        <v>2.359</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G2:G13">
     <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update cnn 48 label result
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343CB33C-029B-45E5-8508-79AA51BC99AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5567BD7-07B5-4C89-B6E0-CEF0FA03C3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="48label_baseline" sheetId="5" r:id="rId5"/>
     <sheet name="48label_ros" sheetId="6" r:id="rId6"/>
     <sheet name="48label_word2vec" sheetId="7" r:id="rId7"/>
+    <sheet name="48label_cnn" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="192">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -616,6 +617,82 @@
   </si>
   <si>
     <t>1 hrs 16 mins 4 secs</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn1filter234drop3 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn1filter234drop5 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn1filter345drop3 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn1filter345drop5 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn2filter234drop3 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn2filter234drop5 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn2filter345drop3 none</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn2filter345drop5 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn1filter234drop3 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn1filter234drop5 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn1filter345drop3 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn1filter345drop5 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn2filter234drop3 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn2filter234drop5 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn2filter345drop3 none</t>
+  </si>
+  <si>
+    <t>roberta-base cnn2filter345drop5 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn1filter234drop3 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn1filter234drop5 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn1filter345drop3 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn1filter345drop5 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn2filter234drop3 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn2filter234drop5 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn2filter345drop3 none</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn2filter345drop5 none</t>
+  </si>
+  <si>
+    <t>train_loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -699,7 +776,14 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1804,34 +1888,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="35" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="36" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="34" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="35" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="33" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="34" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="32" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="33" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="31" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="32" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="30" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="31" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="29" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="30" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="28" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="29" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="27" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="28" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="26" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="27" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1843,7 +1927,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2358,16 +2442,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B25">
-    <cfRule type="top10" dxfId="25" priority="4" rank="5"/>
+    <cfRule type="top10" dxfId="26" priority="4" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="top10" dxfId="24" priority="3" rank="5"/>
+    <cfRule type="top10" dxfId="25" priority="3" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F25">
-    <cfRule type="top10" dxfId="23" priority="2" rank="5"/>
+    <cfRule type="top10" dxfId="24" priority="2" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G25">
-    <cfRule type="top10" dxfId="22" priority="1" rank="5"/>
+    <cfRule type="top10" dxfId="23" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2818,10 +2902,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="21" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="22" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="20" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="21" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3403,34 +3487,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="19" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="20" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="18" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="19" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="17" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="18" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="16" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="17" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="15" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="16" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="14" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="15" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="13" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="14" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="12" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="13" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="11" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="12" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="10" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="11" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3954,25 +4038,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="9" priority="7" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="7" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="8" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="9" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="7" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="8" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="6" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="7" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="5" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="6" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="4" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="5" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="3" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="4" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4461,10 +4545,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="2" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="3" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4475,7 +4559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E03F8-CCBA-4CA7-B914-11C40186E5A7}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -4955,6 +5039,531 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G2:G13">
+    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E17CF8C-6CA7-44C1-B537-933EFCC02AFF}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0.64439999999999997</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.63319999999999999</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.40910000000000002</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.52780000000000005</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.22989999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.65449999999999997</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.64319999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.41060000000000002</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.5444</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.19189999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.64219999999999999</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.40560000000000002</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.54249999999999998</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.19919999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.65190000000000003</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.4204</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.54010000000000002</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.1656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.64549999999999996</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.40570000000000001</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.5323</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.64059999999999995</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.63629999999999998</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.37969999999999998</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.53149999999999997</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.3095</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.65090000000000003</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.63929999999999998</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.53759999999999997</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.21290000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.64510000000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.52859999999999996</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.1802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.52590000000000003</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.2437</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.6371</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.62219999999999998</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.3584</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.38950000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.64049999999999996</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.629</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.39029999999999998</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.52510000000000001</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.30259999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.63149999999999995</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.3911</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.52210000000000001</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.3226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.57369999999999999</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.498</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.21329999999999999</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.34139999999999998</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.2371000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.46779999999999999</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.1517</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1.4414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.60919999999999996</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.59289999999999998</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.2913</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.4849</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.59089999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.43869999999999998</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.26540000000000002</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.7483</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.58650000000000002</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.55220000000000002</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.2868</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.75419999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.5595</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.48420000000000002</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.1918</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.30009999999999998</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1.4823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.62170000000000003</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.3523</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.49509999999999998</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.33250000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.54159999999999997</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.43990000000000001</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1.6876</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.60460000000000003</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.3659</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.55520000000000003</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.47160000000000002</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.14219999999999999</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.32819999999999999</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1.5825</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.53620000000000001</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="D24" s="9">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.31869999999999998</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1.7824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.50209999999999999</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.14979999999999999</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.38490000000000002</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1.2734000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update result and adjust cnn config
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5567BD7-07B5-4C89-B6E0-CEF0FA03C3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38422C-553D-4B56-9E2B-8460D00E944F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="48label_ros" sheetId="6" r:id="rId6"/>
     <sheet name="48label_word2vec" sheetId="7" r:id="rId7"/>
     <sheet name="48label_cnn" sheetId="8" r:id="rId8"/>
+    <sheet name="48label_word2vec+eda" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -693,6 +694,78 @@
   <si>
     <t>train_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bert-base-uncased None word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 44 mins 52 secs</t>
+  </si>
+  <si>
+    <t>bert-base-uncased cnn word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 35 mins 10 secs</t>
+  </si>
+  <si>
+    <t>bert-base-uncased lstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 58 mins 42 secs</t>
+  </si>
+  <si>
+    <t>bert-base-uncased bilstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 52 mins 53 secs</t>
+  </si>
+  <si>
+    <t>roberta-base None word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 47 mins 25 secs</t>
+  </si>
+  <si>
+    <t>roberta-base cnn word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 49 mins 14 secs</t>
+  </si>
+  <si>
+    <t>roberta-base lstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>1 hrs 11 mins 13 secs</t>
+  </si>
+  <si>
+    <t>roberta-base bilstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>1 hrs 11 mins 18 secs</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base None word2vec_eda</t>
+  </si>
+  <si>
+    <t>1 hrs 7 mins 53 secs</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base cnn word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 55 mins 11 secs</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base lstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>0 hrs 35 mins 13 secs</t>
+  </si>
+  <si>
+    <t>microsoft/deberta-base bilstm word2vec_eda</t>
+  </si>
+  <si>
+    <t>1 hrs 40 mins 4 secs</t>
   </si>
 </sst>
 </file>
@@ -776,7 +849,14 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1888,34 +1968,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="36" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="37" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="35" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="36" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="34" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="35" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="33" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="34" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="32" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="33" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="31" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="32" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="30" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="31" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="29" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="30" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="28" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="29" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="27" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="28" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2442,16 +2522,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B25">
-    <cfRule type="top10" dxfId="26" priority="4" rank="5"/>
+    <cfRule type="top10" dxfId="27" priority="4" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="top10" dxfId="25" priority="3" rank="5"/>
+    <cfRule type="top10" dxfId="26" priority="3" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F25">
-    <cfRule type="top10" dxfId="24" priority="2" rank="5"/>
+    <cfRule type="top10" dxfId="25" priority="2" rank="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G25">
-    <cfRule type="top10" dxfId="23" priority="1" rank="5"/>
+    <cfRule type="top10" dxfId="24" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2902,10 +2982,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="22" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="23" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="21" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="22" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3487,34 +3567,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="20" priority="10" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="21" priority="10" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="19" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="20" priority="9" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="18" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="19" priority="8" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="17" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="18" priority="7" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="16" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="17" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="15" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="16" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I13">
-    <cfRule type="top10" dxfId="14" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="15" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J13">
-    <cfRule type="top10" dxfId="13" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="14" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M13">
-    <cfRule type="top10" dxfId="12" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="13" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N13">
-    <cfRule type="top10" dxfId="11" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="12" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4038,25 +4118,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="10" priority="7" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="11" priority="7" bottom="1" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="9" priority="6" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="6" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="top10" dxfId="8" priority="5" rank="3"/>
+    <cfRule type="top10" dxfId="9" priority="5" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="7" priority="4" rank="3"/>
+    <cfRule type="top10" dxfId="8" priority="4" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="6" priority="3" rank="3"/>
+    <cfRule type="top10" dxfId="7" priority="3" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="5" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="6" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="top10" dxfId="4" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="5" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4545,10 +4625,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="3" priority="2" rank="3"/>
+    <cfRule type="top10" dxfId="4" priority="2" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="2" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="3" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4560,7 +4640,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5039,7 +5119,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5051,7 +5131,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5564,6 +5644,497 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D25">
+    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDAE853-41FD-426B-83A6-86030E6D9E5C}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1.7633318481648801</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.63773534445870705</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.64585828517214805</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.63773534445870705</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.63209686587194303</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.42266767856564602</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.424866302265412</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.52335837026211496</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.15858271169754501</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1.6060506546642701</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.64292141076445097</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.64788097263192801</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.64292141076445097</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.62880265308775896</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.419193447998292</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.41426456144062401</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.522161283524194</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.41292034835052499</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1.7065480208978401</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.64231072445163795</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.64914280521756695</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.64231072445163795</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.63456516154213005</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.41642881057056802</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.42394526186094</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.52965118805703404</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.280976879672932</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1.6844555593527299</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.64170271250767397</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.65118305208096705</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.64170271250767397</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.63679617815674805</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.41874004653369301</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.42851655284519002</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.52903004661683195</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.261424004426486</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2.02518721718977</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.60158369146620505</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.56010813354540401</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.60158369146620505</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.56306214712604796</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.33591177116505999</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.33577325471428998</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.41325757668533702</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.91616751128435603</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1.7286468746821999</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.62583742628044103</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.64314354051438005</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.62583742628044103</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.62471608290857195</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.40170177814221403</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.41503025460943599</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.51124042310741102</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.33378010952758003</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.66500821949505</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.59991162955107802</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.62326123009955003</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.59991162955107802</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.59561874325319897</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.37842957103013303</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.39554160615859202</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.47365818700672502</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.701845622032506</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1.6963374429723099</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.60921250302319896</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.63388463041651699</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.60921250302319896</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.609708652447846</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.39908908887107902</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.41791952793020198</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.490704431636454</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.50646139980168903</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" s="10">
+        <v>2.30053117048086</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.59608949135830003</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.55361795674316705</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.59608949135830003</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.55691609611373105</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.33008068820880498</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.33489385401965799</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.40843403254931898</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.82586389531957105</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2.09086211956128</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.59258804487358296</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.56358777540334104</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.59258804487358296</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.55670726127855996</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.32178395353003297</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.33476428167644501</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.42888508012367699</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1.03129530288474</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="10">
+        <v>2.7874045825586</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.45393260125392998</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.28674363044323398</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.45393260125392998</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.34138126396280599</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2.6233249079102398E-2</v>
+      </c>
+      <c r="H12" s="10">
+        <v>4.7457167005305903E-2</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.13642573046380399</v>
+      </c>
+      <c r="J12" s="10">
+        <v>3.4645091849998302</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2.3795432114019599</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.51372544231735195</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.48977421624057998</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.51372544231735195</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.48758786597237003</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.214164303979616</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.233778361020088</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.33398580589150201</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1.42454044189455</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update lstm ablation study
</commit_message>
<xml_diff>
--- a/experiment_result/result.xlsx
+++ b/experiment_result/result.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Jupyter\aiops\experiment_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38422C-553D-4B56-9E2B-8460D00E944F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3924A9-AD19-417B-8253-F1506F97E58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
     <sheet name="cnn" sheetId="3" r:id="rId2"/>
     <sheet name="word2vec" sheetId="4" r:id="rId3"/>
-    <sheet name="resampling" sheetId="2" r:id="rId4"/>
-    <sheet name="48label_baseline" sheetId="5" r:id="rId5"/>
-    <sheet name="48label_ros" sheetId="6" r:id="rId6"/>
-    <sheet name="48label_word2vec" sheetId="7" r:id="rId7"/>
-    <sheet name="48label_cnn" sheetId="8" r:id="rId8"/>
+    <sheet name="48label_cnn" sheetId="8" r:id="rId4"/>
+    <sheet name="resampling" sheetId="2" r:id="rId5"/>
+    <sheet name="48label_baseline" sheetId="5" r:id="rId6"/>
+    <sheet name="48label_ros" sheetId="6" r:id="rId7"/>
+    <sheet name="48label_word2vec" sheetId="7" r:id="rId8"/>
     <sheet name="48label_word2vec+eda" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="215">
   <si>
     <t>val_loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,42 +584,6 @@
     <t>1 hrs 19 mins 13 secs</t>
   </si>
   <si>
-    <t>0 hrs 46 mins 16 secs</t>
-  </si>
-  <si>
-    <t>0 hrs 45 mins 8 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 3 mins 3 secs</t>
-  </si>
-  <si>
-    <t>0 hrs 48 mins 14 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 5 mins 50 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 5 mins 47 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 13 mins 14 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 32 mins 41 secs</t>
-  </si>
-  <si>
-    <t>0 hrs 52 mins 47 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 5 mins 15 secs</t>
-  </si>
-  <si>
-    <t>0 hrs 53 mins 35 secs</t>
-  </si>
-  <si>
-    <t>1 hrs 16 mins 4 secs</t>
-  </si>
-  <si>
     <t>bert-base-uncased cnn1filter234drop3 none</t>
   </si>
   <si>
@@ -766,6 +730,39 @@
   </si>
   <si>
     <t>1 hrs 40 mins 4 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 44 mins 30 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 36 mins 45 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 46 mins 18 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 59 mins 47 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 58 mins 7 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 40 mins 35 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 5 mins 11 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 2 mins 59 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 57 mins 49 secs</t>
+  </si>
+  <si>
+    <t>0 hrs 55 mins 56 secs</t>
+  </si>
+  <si>
+    <t>1 hrs 26 mins 8 secs</t>
   </si>
 </sst>
 </file>
@@ -2993,6 +2990,531 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E17CF8C-6CA7-44C1-B537-933EFCC02AFF}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0.64439999999999997</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.63319999999999999</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.40910000000000002</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.52780000000000005</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.22989999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.65449999999999997</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.64319999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.41060000000000002</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.5444</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.19189999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.64219999999999999</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.40560000000000002</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.54249999999999998</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.19919999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.65190000000000003</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.4204</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.54010000000000002</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.1656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.64549999999999996</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.40570000000000001</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.5323</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.64059999999999995</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.63629999999999998</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.37969999999999998</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.53149999999999997</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.3095</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.65090000000000003</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.63929999999999998</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.53759999999999997</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.21290000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.64510000000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.52859999999999996</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.1802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.63</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.52590000000000003</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.2437</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.6371</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.62219999999999998</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.3584</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.38950000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.64049999999999996</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.629</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.39029999999999998</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.52510000000000001</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.30259999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0.63349999999999995</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.63149999999999995</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.3911</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.52210000000000001</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.3226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.57369999999999999</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.498</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.21329999999999999</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.34139999999999998</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.2371000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.46779999999999999</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.1517</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1.4414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.60919999999999996</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.59289999999999998</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.2913</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.4849</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.59089999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.43869999999999998</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.26540000000000002</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.7483</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.58650000000000002</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.55220000000000002</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.2868</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.75419999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.5595</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.48420000000000002</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.1918</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.30009999999999998</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1.4823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.62170000000000003</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.3523</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.49509999999999998</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.33250000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0.54159999999999997</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.43990000000000001</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1.6876</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0.60460000000000003</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.32140000000000002</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.3659</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.55520000000000003</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.47160000000000002</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.14219999999999999</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.32819999999999999</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1.5825</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.53620000000000001</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="D24" s="9">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.31869999999999998</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1.7824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.50209999999999999</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.14979999999999999</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.38490000000000002</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1.2734000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2:D25">
+    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03916FF-E967-4F88-8D67-A577C87F376D}">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -3601,7 +4123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B2AF50-4881-4BD8-ABC8-BC15E9EA58C5}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -4143,7 +4665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65FADA8-07B8-4272-9C6D-6AA1D1013DC4}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -4635,12 +5157,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E03F8-CCBA-4CA7-B914-11C40186E5A7}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4649,14 +5171,14 @@
     <col min="2" max="2" width="8.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -4697,423 +5219,459 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="5">
-        <v>1.8025</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.63619999999999999</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.64449999999999996</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.63619999999999999</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.62970000000000004</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.4234</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.42030000000000001</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.52249999999999996</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.25929999999999997</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>155</v>
+      <c r="B2" s="10">
+        <v>1.7481197245600699</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.64490893192684795</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.64675678977135098</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.64490893192684795</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.63476631412295004</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.422908955880962</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.42770990864831798</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.53211581554232201</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.24482818922862301</v>
+      </c>
+      <c r="K2" s="9">
+        <v>2670</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="5">
-        <v>1.7537</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.65069999999999995</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.6462</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.65069999999999995</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.63790000000000002</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.43090000000000001</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.42770000000000002</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.53449999999999998</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.18310000000000001</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>156</v>
+      <c r="B3" s="10">
+        <v>1.68291767319528</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.63285834217037795</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.64821631790761702</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.63285834217037795</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.63006120848784697</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.42377712783777799</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.44217614209678402</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.523715843583064</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.31850661056066798</v>
+      </c>
+      <c r="K3" s="9">
+        <v>2205</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="5">
-        <v>1.6760999999999999</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.64490000000000003</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.63929999999999998</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.64490000000000003</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.63129999999999997</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.41770000000000002</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.52380000000000004</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.27260000000000001</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>157</v>
+      <c r="B4" s="10">
+        <v>1.5862721682685099</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.63392541534110902</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.63485128485907605</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.63392541534110902</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.62657562520368904</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.42110039498712998</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.43055737074824701</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.51696893769277397</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.41581065463339201</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2778</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="5">
-        <v>1.5810999999999999</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.65480000000000005</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.64590000000000003</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.65480000000000005</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.63829999999999998</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.41539999999999999</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.40379999999999999</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.53700000000000003</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.37169999999999997</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>158</v>
+      <c r="B5" s="10">
+        <v>1.7879512322748501</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.64093842440140603</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.65148878050164305</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.64093842440140603</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.63547513895813401</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.42718657106232899</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.42386455573653797</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.527328518270053</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.15341508413018501</v>
+      </c>
+      <c r="K5" s="9">
+        <v>3587</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="5">
-        <v>1.9300999999999999</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.6411</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.6421</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.6411</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.63260000000000005</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.41820000000000002</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.42049999999999998</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.52569999999999995</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.1636</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>159</v>
+      <c r="B6" s="10">
+        <v>1.9077054051228</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.62889050901378496</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.64549111044995899</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.62889050901378496</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.62620842167595403</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.42111271659613903</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.43335333242309398</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.51268683288518002</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.19479241613714801</v>
+      </c>
+      <c r="K6" s="9">
+        <v>3487</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="5">
-        <v>1.8488</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.64049999999999996</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.64449999999999996</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.64049999999999996</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.40760000000000002</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.41460000000000002</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.52549999999999997</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0.17119999999999999</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>160</v>
+      <c r="B7" s="10">
+        <v>2.0257840923056301</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.57717716879685899</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.55868684322088902</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.57717716879685899</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.55171551467184499</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.32959119356403999</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.35484302087203501</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.41358547358292702</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1.01361543935009</v>
+      </c>
+      <c r="K7" s="9">
+        <v>2435</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="5">
-        <v>1.6679999999999999</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.60909999999999997</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.61570000000000003</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.60909999999999997</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.59260000000000002</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.3735</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.3952</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.4748</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.7036</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>161</v>
+      <c r="B8" s="10">
+        <v>1.91106558696525</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.57185994214061098</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.549885603895512</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.57185994214061098</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.54355158871879805</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.32109765438117199</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.34858545990265299</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.40200365197064603</v>
+      </c>
+      <c r="J8" s="10">
+        <v>1.1627840690319899</v>
+      </c>
+      <c r="K8" s="9">
+        <v>3911</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="5">
-        <v>1.8138000000000001</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.59460000000000002</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.61850000000000005</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.59460000000000002</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.59079999999999999</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.38159999999999999</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.39510000000000001</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.4708</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.44080000000000003</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>162</v>
+      <c r="B9" s="10">
+        <v>2.0355511979358898</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.57672240981563105</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.55737834921163598</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.57672240981563105</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.55500330373278794</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.31374916139575998</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.32993851461663698</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.42371495433915801</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.92596363917516</v>
+      </c>
+      <c r="K9" s="9">
+        <v>3779</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="5">
-        <v>2.0933999999999999</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0.58509999999999995</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.55069999999999997</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.58509999999999995</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.31669999999999998</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.33289999999999997</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.40150000000000002</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.97460000000000002</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>163</v>
+      <c r="B10" s="10">
+        <v>2.22592040496628</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.60036022585626303</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.553536488582557</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.60036022585626303</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.56174149873694201</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.32582058314353102</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.33127435772620301</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.41669358995198003</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.82395546536355402</v>
+      </c>
+      <c r="K10" s="9">
+        <v>3469</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="5">
-        <v>2.214</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.6008</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.55269999999999997</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.6008</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.56059999999999999</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.32879999999999998</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.32550000000000001</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.41310000000000002</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.8306</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>164</v>
+      <c r="B11" s="10">
+        <v>2.4531468331268602</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.56619074528845903</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.470994602220554</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.56619074528845903</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.49540097374180497</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.25238910988769703</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.25735463977414702</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.30984738749618101</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1.5735375735069701</v>
+      </c>
+      <c r="K11" s="9">
+        <v>3356</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="5">
-        <v>2.4234</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0.46829999999999999</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.3589</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.46829999999999999</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="G12" s="4">
-        <v>6.59E-2</v>
-      </c>
-      <c r="H12" s="5">
-        <v>9.69E-2</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.221</v>
-      </c>
-      <c r="J12" s="5">
-        <v>2.8668999999999998</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>165</v>
+      <c r="B12" s="10">
+        <v>2.5546596561990098</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.45684882606835198</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.33400823395263102</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.45684882606835198</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.36841695927265999</v>
+      </c>
+      <c r="G12" s="10">
+        <v>4.4919909831794801E-2</v>
+      </c>
+      <c r="H12" s="10">
+        <v>7.0884573865882594E-2</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.18152850403985599</v>
+      </c>
+      <c r="J12" s="10">
+        <v>3.2241955172416201</v>
+      </c>
+      <c r="K12" s="9">
+        <v>2110</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="5">
-        <v>2.3544999999999998</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.4965</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.41360000000000002</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.4965</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.43380000000000002</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.12989999999999999</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.15679999999999999</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.27560000000000001</v>
-      </c>
-      <c r="J13" s="5">
-        <v>2.359</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>166</v>
+      <c r="B13" s="10">
+        <v>2.3901268480027502</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.49619890792729399</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.43593042031661999</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.49619890792729399</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.44671973667531401</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.164489625284619</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.191639308133947</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.291015861103674</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1.9436613104748399</v>
+      </c>
+      <c r="K13" s="9">
+        <v>5168</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5126,537 +5684,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E17CF8C-6CA7-44C1-B537-933EFCC02AFF}">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="9">
-        <v>0.64439999999999997</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0.63319999999999999</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.40910000000000002</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.52780000000000005</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0.22989999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0.65449999999999997</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0.64319999999999999</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.41060000000000002</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.5444</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.19189999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.64219999999999999</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.40560000000000002</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0.54249999999999998</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0.19919999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0.65190000000000003</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.64290000000000003</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.4204</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0.54010000000000002</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.1656</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0.64549999999999996</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.40570000000000001</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0.5323</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.64059999999999995</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0.63629999999999998</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.37969999999999998</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0.53149999999999997</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0.3095</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0.65090000000000003</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0.63929999999999998</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0.53759999999999997</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.21290000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0.64510000000000001</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0.63419999999999999</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.39529999999999998</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0.52859999999999996</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0.1802</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.64</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.63</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.52590000000000003</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.2437</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.6371</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0.62219999999999998</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.3584</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.51859999999999995</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.38950000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0.64049999999999996</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0.629</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.39029999999999998</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.52510000000000001</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.30259999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0.63349999999999995</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0.63149999999999995</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.3911</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.52210000000000001</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.3226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0.57369999999999999</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0.498</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.21329999999999999</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0.34139999999999998</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1.2371000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0.55430000000000001</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0.46779999999999999</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.1517</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="F15" s="9">
-        <v>1.4414</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0.60919999999999996</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0.59289999999999998</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.2913</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0.4849</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0.59089999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="9">
-        <v>0.53690000000000004</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0.43869999999999998</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.12139999999999999</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0.26540000000000002</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1.7483</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B18" s="9">
-        <v>0.58650000000000002</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0.55220000000000002</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0.2868</v>
-      </c>
-      <c r="E18" s="9">
-        <v>0.40250000000000002</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0.75419999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="9">
-        <v>0.5595</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0.48420000000000002</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0.1918</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.30009999999999998</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1.4823</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B20" s="9">
-        <v>0.62170000000000003</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0.60770000000000002</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0.3523</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0.49509999999999998</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0.33250000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B21" s="9">
-        <v>0.54159999999999997</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0.43990000000000001</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.15709999999999999</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0.24629999999999999</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1.6876</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B22" s="9">
-        <v>0.60460000000000003</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0.60050000000000003</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0.32140000000000002</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0.48480000000000001</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0.3659</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="B23" s="9">
-        <v>0.55520000000000003</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0.47160000000000002</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0.14219999999999999</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0.32819999999999999</v>
-      </c>
-      <c r="F23" s="9">
-        <v>1.5825</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0.53620000000000001</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0.44040000000000001</v>
-      </c>
-      <c r="D24" s="9">
-        <v>9.7600000000000006E-2</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.31869999999999998</v>
-      </c>
-      <c r="F24" s="9">
-        <v>1.7824</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="B25" s="9">
-        <v>0.55430000000000001</v>
-      </c>
-      <c r="C25" s="9">
-        <v>0.50209999999999999</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0.14979999999999999</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0.38490000000000002</v>
-      </c>
-      <c r="F25" s="9">
-        <v>1.2734000000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D25">
-    <cfRule type="top10" dxfId="1" priority="1" rank="3"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDAE853-41FD-426B-83A6-86030E6D9E5C}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5714,7 +5747,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B2" s="10">
         <v>1.7633318481648801</v>
@@ -5744,12 +5777,12 @@
         <v>0.15858271169754501</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B3" s="10">
         <v>1.6060506546642701</v>
@@ -5779,12 +5812,12 @@
         <v>0.41292034835052499</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B4" s="10">
         <v>1.7065480208978401</v>
@@ -5814,12 +5847,12 @@
         <v>0.280976879672932</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B5" s="10">
         <v>1.6844555593527299</v>
@@ -5849,12 +5882,12 @@
         <v>0.261424004426486</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B6" s="10">
         <v>2.02518721718977</v>
@@ -5884,12 +5917,12 @@
         <v>0.91616751128435603</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B7" s="10">
         <v>1.7286468746821999</v>
@@ -5919,12 +5952,12 @@
         <v>0.33378010952758003</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B8" s="10">
         <v>1.66500821949505</v>
@@ -5954,12 +5987,12 @@
         <v>0.701845622032506</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B9" s="10">
         <v>1.6963374429723099</v>
@@ -5989,12 +6022,12 @@
         <v>0.50646139980168903</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B10" s="10">
         <v>2.30053117048086</v>
@@ -6024,12 +6057,12 @@
         <v>0.82586389531957105</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B11" s="10">
         <v>2.09086211956128</v>
@@ -6059,12 +6092,12 @@
         <v>1.03129530288474</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B12" s="10">
         <v>2.7874045825586</v>
@@ -6094,12 +6127,12 @@
         <v>3.4645091849998302</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B13" s="10">
         <v>2.3795432114019599</v>
@@ -6129,7 +6162,7 @@
         <v>1.42454044189455</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>